<commit_message>
fixed some login issues
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1102a251f21c2137/Professional/Jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saman\Documents\Git\job-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B8471000-4754-4112-95D8-7AA4131B4452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF7BF03C-C73A-4ABA-BB17-68E9402DC131}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6439116A-A2B4-4E6E-AEDD-BE2B20740C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-21600" windowWidth="19290" windowHeight="11230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="311">
   <si>
     <t>Company</t>
   </si>
@@ -944,6 +944,15 @@
   </si>
   <si>
     <t>https://www.sparkmicro.com/careers/</t>
+  </si>
+  <si>
+    <t>Ericsson</t>
+  </si>
+  <si>
+    <t>ASIC Architect</t>
+  </si>
+  <si>
+    <t>https://jobs.ericsson.com/careers/job/563121765371416</t>
   </si>
 </sst>
 </file>
@@ -1323,11 +1332,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2807,6 +2816,26 @@
       </c>
       <c r="F64" s="2" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>308</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" t="s">
+        <v>309</v>
+      </c>
+      <c r="E65">
+        <v>768407</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2871,8 +2900,9 @@
     <hyperlink ref="F61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
     <hyperlink ref="F62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
     <hyperlink ref="F64" r:id="rId60" xr:uid="{BDDF334D-5E91-484B-AC44-FCBEFBCFB89D}"/>
+    <hyperlink ref="F65" r:id="rId61" xr:uid="{A4AB8551-B240-457F-AEA0-8634D7D52B06}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId61"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>